<commit_message>
Updating docs to Version 1.0.1 Changes:    * Adding required field to all definitions RT:530380    * Updating code 4 on Principal Focus of Treatment RT:530677    * Adding response code 0 to Income Source RT:530704
</commit_message>
<xml_diff>
--- a/doc/build/html/_static/pmhc-upload.xlsx
+++ b/doc/build/html/_static/pmhc-upload.xlsx
@@ -2330,10 +2330,10 @@
         <v>2</v>
       </c>
       <c r="AN3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AO3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AP3">
         <v>0</v>
@@ -2345,16 +2345,16 @@
         <v>2</v>
       </c>
       <c r="AS3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AT3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AU3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AV3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AW3">
         <v>99</v>

</xml_diff>